<commit_message>
added  new empty sheet
</commit_message>
<xml_diff>
--- a/pandas/data/tableXL.xlsx
+++ b/pandas/data/tableXL.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\work\WorkN\ReadExcel\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\work\WorkN\PythonNotesToSelf\pandas\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,8 @@
   <sheets>
     <sheet name="NAR18A" sheetId="7" state="hidden" r:id="rId1"/>
     <sheet name="BTOL 18A" sheetId="11" state="hidden" r:id="rId2"/>
-    <sheet name="table" sheetId="17" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="18" r:id="rId3"/>
+    <sheet name="table" sheetId="17" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
@@ -2799,11 +2800,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="451156632"/>
-        <c:axId val="451157024"/>
+        <c:axId val="208699568"/>
+        <c:axId val="168693592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="451156632"/>
+        <c:axId val="208699568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2816,12 +2817,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="451157024"/>
+        <c:crossAx val="168693592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="451157024"/>
+        <c:axId val="168693592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2832,7 +2833,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="451156632"/>
+        <c:crossAx val="208699568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -16395,9 +16396,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="U5:AG32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+    <sheetView topLeftCell="R4" workbookViewId="0">
       <selection activeCell="AG7" sqref="AG7"/>
     </sheetView>
   </sheetViews>

</xml_diff>